<commit_message>
this iss the Client Test Plan
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6210"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global Test" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>Login Page</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Fill out everything correctlly with a new user name</t>
   </si>
   <si>
-    <t>The user is braught back to the login screen and he or she is able to log in with the new login credentials.</t>
-  </si>
-  <si>
     <t>Verify that the "First Name","Last Name", "Acqaintancce ID", "Relation", and "Message" fields are present. Along with picture 1,2, 3 buttons and Add Button</t>
   </si>
   <si>
@@ -264,6 +261,15 @@
   </si>
   <si>
     <t>This Test should work simular to single capture mode, but the user should not ned to manually take the picture</t>
+  </si>
+  <si>
+    <t>The user is braught back to the login screen and he or she is able to log in with the new login credentials. The user is also sent a verification email that he or she needs to accept before he or she can log in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that the email arrives.</t>
+  </si>
+  <si>
+    <t>Verify that after clicking th link in the email the user is able to log into the app</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -932,14 +938,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,27 +1024,35 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1529,7 +1543,7 @@
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>39</v>
@@ -1541,7 +1555,7 @@
     </row>
     <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>39</v>
@@ -1553,10 +1567,10 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1565,10 +1579,10 @@
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1577,10 +1591,10 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1589,10 +1603,10 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1601,10 +1615,10 @@
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1760,7 +1774,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>39</v>
@@ -1780,10 +1794,10 @@
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1800,10 +1814,10 @@
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1820,10 +1834,10 @@
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1840,10 +1854,10 @@
     </row>
     <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2286,7 +2300,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>39</v>
@@ -2299,7 +2313,7 @@
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>39</v>

</xml_diff>